<commit_message>
Update Avaliação dos modelos.xlsx
</commit_message>
<xml_diff>
--- a/Evaluation/Avaliação dos modelos.xlsx
+++ b/Evaluation/Avaliação dos modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/fabio_cordeiro_petrobras_com_br/Documents/Documents/Repositorios/Petro_KGraph/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="11_F25DC773A252ABDACC1048D6215F78F25ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7026F17B-FA79-408D-9DA7-DB00EACE7CC4}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="11_F25DC773A252ABDACC1048D6215F78F25ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46F8F447-08B1-4308-B652-E453C8F14658}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1845" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PetroVec" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Modelo NER" sheetId="1" r:id="rId4"/>
     <sheet name="Modelo Instances clustering" sheetId="2" r:id="rId5"/>
     <sheet name="Modelo RE" sheetId="3" r:id="rId6"/>
+    <sheet name="Pipeline" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="181">
   <si>
     <t>Baseline</t>
   </si>
@@ -47,15 +48,9 @@
     <t>Modelo BERT pretreinado</t>
   </si>
   <si>
-    <t>"neuralmind/bert-large-portuguese-cased"</t>
-  </si>
-  <si>
     <t>Arquitetura</t>
   </si>
   <si>
-    <t>Sentence (input_id, attention_masks); tf_bert_model; dropout(0.3); dense(softmax)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Loss function </t>
   </si>
   <si>
@@ -203,9 +198,6 @@
     <t>"neuralmind/bert-base-portuguese-cased"</t>
   </si>
   <si>
-    <t>Sentence (input_id, attention_masks); tf_bert_model; dropout(0.1); dense(64, 'relu'); dense(softmax)</t>
-  </si>
-  <si>
     <t>CategoricalCrossentropy</t>
   </si>
   <si>
@@ -236,12 +228,6 @@
     <t>PetroVec</t>
   </si>
   <si>
-    <t>Petrovec-OeG-100</t>
-  </si>
-  <si>
-    <t>Petrovec-híbrido-100</t>
-  </si>
-  <si>
     <t>Descrição</t>
   </si>
   <si>
@@ -275,12 +261,6 @@
     <t>Corpora-size</t>
   </si>
   <si>
-    <t>Petrovec-OeG_NP2-100</t>
-  </si>
-  <si>
-    <t>Petrovec-híbrido_NP2-100</t>
-  </si>
-  <si>
     <t>ontology_file = ../../KnowledgeGraph/OntoGeoLogicaInstanciasRelacoes.owl</t>
   </si>
   <si>
@@ -450,6 +430,150 @@
   </si>
   <si>
     <t>treinando</t>
+  </si>
+  <si>
+    <t>Petrovec-OeG-pub</t>
+  </si>
+  <si>
+    <t>Petrovec-híbrido_pub-NP2</t>
+  </si>
+  <si>
+    <t>Petrovec-híbrido-pub</t>
+  </si>
+  <si>
+    <t>Petrovec-OeG_pub-NP2</t>
+  </si>
+  <si>
+    <t>Bertimbau Large</t>
+  </si>
+  <si>
+    <t>Baseline-0</t>
+  </si>
+  <si>
+    <t>DEPS (UPOS) como input</t>
+  </si>
+  <si>
+    <t>Sentence (input_id, attention_masks); tf_bert_model; dropout(0.1); dense(softmax)</t>
+  </si>
+  <si>
+    <t>Dropout_03</t>
+  </si>
+  <si>
+    <t>TinyBert</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>Alpha 01</t>
+  </si>
+  <si>
+    <t>Alpha 001</t>
+  </si>
+  <si>
+    <t>Augmented F1-Score</t>
+  </si>
+  <si>
+    <t>Augmented Precision</t>
+  </si>
+  <si>
+    <t>Augmented Recall</t>
+  </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <t>PetroOntoVec</t>
+  </si>
+  <si>
+    <t>Modelo NER</t>
+  </si>
+  <si>
+    <t>Modelo Intances Clustering</t>
+  </si>
+  <si>
+    <t>Modelo RE</t>
+  </si>
+  <si>
+    <t>Jaccard Geral</t>
+  </si>
+  <si>
+    <t>bacia</t>
+  </si>
+  <si>
+    <t>campo</t>
+  </si>
+  <si>
+    <t>estrutura</t>
+  </si>
+  <si>
+    <t>poco</t>
+  </si>
+  <si>
+    <t>textura</t>
+  </si>
+  <si>
+    <t>lito</t>
+  </si>
+  <si>
+    <t>tempo_geo</t>
+  </si>
+  <si>
+    <t>rocha</t>
+  </si>
+  <si>
+    <t>uncosol</t>
+  </si>
+  <si>
+    <t>og_fluid</t>
+  </si>
+  <si>
+    <t>earth_fluid</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>sistema_petro</t>
+  </si>
+  <si>
+    <t>elemento_petro</t>
+  </si>
+  <si>
+    <t>qualidade_tempo_geo</t>
+  </si>
+  <si>
+    <t>crosses</t>
+  </si>
+  <si>
+    <t>participates_in</t>
+  </si>
+  <si>
+    <t>part_of</t>
+  </si>
+  <si>
+    <t>carrier_of</t>
+  </si>
+  <si>
+    <t>generated_by</t>
+  </si>
+  <si>
+    <t>has_temporal_relation</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Base Classes</t>
+  </si>
+  <si>
+    <t>instance Clustering scores usando parâmetros do modelos base</t>
+  </si>
+  <si>
+    <t>10 com patience= 5 (melhor val_loss na epoch = 3)</t>
+  </si>
+  <si>
+    <t>10 com patience= 5 (melhor val_loss na epoch =  )</t>
   </si>
 </sst>
 </file>
@@ -803,7 +927,7 @@
   <dimension ref="A2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,33 +942,33 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -859,15 +983,15 @@
         <v>85725834</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -882,15 +1006,15 @@
         <v>365295169</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -899,15 +1023,15 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -916,7 +1040,7 @@
         <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -926,800 +1050,836 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C6100A-D7AE-4C72-AEAD-5A5CC55A8794}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="5" width="31.77734375" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" customWidth="1"/>
-    <col min="7" max="10" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="6" width="31.77734375" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="11" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>113</v>
-      </c>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>83</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C10" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D10" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E10" t="s">
         <v>83</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F10" t="s">
         <v>83</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G10" t="s">
         <v>83</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H10" t="s">
         <v>83</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I10" t="s">
         <v>83</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J10" t="s">
         <v>83</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>84</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D11" t="s">
         <v>84</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E11" t="s">
         <v>84</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F11" t="s">
         <v>84</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G11" t="s">
         <v>84</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H11" t="s">
         <v>84</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I11" t="s">
         <v>84</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J11" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="K11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>85</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D12" t="s">
         <v>85</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E12" t="s">
         <v>85</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F12" t="s">
         <v>85</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" t="s">
         <v>85</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I12" t="s">
         <v>85</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J12" t="s">
         <v>85</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K12" t="s">
         <v>85</v>
       </c>
-      <c r="J5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>86</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E13" t="s">
         <v>86</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F13" t="s">
         <v>86</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G13" t="s">
         <v>86</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" t="s">
         <v>86</v>
       </c>
-      <c r="H6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>87</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D14" t="s">
         <v>87</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E14" t="s">
         <v>87</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F14" t="s">
         <v>87</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G14" t="s">
         <v>87</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H14" t="s">
         <v>87</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I14" t="s">
         <v>87</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J14" t="s">
         <v>87</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>88</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D15" t="s">
         <v>88</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E15" t="s">
         <v>88</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G15" t="s">
         <v>88</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H15" t="s">
         <v>88</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I15" t="s">
         <v>88</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J15" t="s">
         <v>88</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>89</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C16" t="s">
         <v>89</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D16" t="s">
         <v>89</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E16" t="s">
         <v>89</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F16" t="s">
         <v>89</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G16" t="s">
         <v>89</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H16" t="s">
         <v>89</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I16" t="s">
         <v>89</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J16" t="s">
         <v>89</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>90</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D17" t="s">
         <v>90</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E17" t="s">
         <v>90</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F17" t="s">
         <v>90</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G17" t="s">
         <v>90</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H17" t="s">
         <v>90</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I17" t="s">
         <v>90</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J17" t="s">
         <v>90</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>91</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" t="s">
         <v>91</v>
       </c>
-      <c r="C11" t="s">
+      <c r="H18" t="s">
         <v>91</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I18" t="s">
         <v>91</v>
       </c>
-      <c r="E11" t="s">
+      <c r="J18" t="s">
         <v>91</v>
       </c>
-      <c r="F11" t="s">
+      <c r="K18" t="s">
         <v>91</v>
       </c>
-      <c r="G11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" t="s">
-        <v>91</v>
-      </c>
-      <c r="J11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>92</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D19" t="s">
         <v>92</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E19" t="s">
         <v>92</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G19" t="s">
         <v>92</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H19" t="s">
         <v>92</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I19" t="s">
         <v>92</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J19" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="K19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>93</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D20" t="s">
         <v>93</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E20" t="s">
         <v>93</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F20" t="s">
         <v>93</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G20" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>94</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C21" t="s">
         <v>94</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D21" t="s">
         <v>94</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E21" t="s">
         <v>94</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F21" t="s">
         <v>94</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G21" t="s">
         <v>94</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H21" t="s">
         <v>94</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I21" t="s">
         <v>94</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J21" t="s">
         <v>94</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D22" t="s">
         <v>95</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E22" t="s">
         <v>95</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F22" t="s">
         <v>95</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G22" t="s">
         <v>95</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H22" t="s">
         <v>95</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I22" t="s">
         <v>95</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J22" t="s">
         <v>95</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>96</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D23" t="s">
         <v>96</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E23" t="s">
         <v>96</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F23" t="s">
         <v>96</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G23" t="s">
         <v>96</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H23" t="s">
         <v>96</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I23" t="s">
         <v>96</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J23" t="s">
         <v>96</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>97</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D24" t="s">
         <v>97</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E24" t="s">
         <v>97</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F24" t="s">
         <v>97</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G24" t="s">
         <v>97</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H24" t="s">
         <v>97</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I24" t="s">
         <v>97</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J24" t="s">
         <v>97</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="G18" t="s">
+      <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="H18" t="s">
+      <c r="E25" t="s">
         <v>98</v>
       </c>
-      <c r="I18" t="s">
+      <c r="F25" t="s">
         <v>98</v>
       </c>
-      <c r="J18" t="s">
+      <c r="G25" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" t="s">
-        <v>100</v>
-      </c>
-      <c r="I20" t="s">
-        <v>100</v>
-      </c>
-      <c r="J20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" t="s">
-        <v>101</v>
-      </c>
-      <c r="I21" t="s">
-        <v>101</v>
-      </c>
-      <c r="J21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" t="s">
-        <v>102</v>
-      </c>
-      <c r="I22" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" t="s">
-        <v>103</v>
-      </c>
-      <c r="I23" t="s">
-        <v>103</v>
-      </c>
-      <c r="J23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" t="s">
-        <v>104</v>
-      </c>
-      <c r="J24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" t="s">
-        <v>105</v>
-      </c>
       <c r="H25" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" t="s">
-        <v>134</v>
+        <v>98</v>
+      </c>
+      <c r="K25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H26" t="s">
-        <v>139</v>
+        <v>127</v>
+      </c>
+      <c r="I26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1729,27 +1889,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80464D9-BE08-48C0-9C57-068FB602ABD8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>135</v>
+      <c r="A1" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -1757,10 +1920,45 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1770,20 +1968,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="29.88671875" customWidth="1"/>
+    <col min="11" max="15" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1794,562 +1994,549 @@
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="B2" s="4">
-        <v>0.80598433998331098</v>
+        <v>0.82705015605171295</v>
       </c>
       <c r="C2" s="4">
-        <v>0.88835645129893404</v>
+        <v>0.77951575564926801</v>
       </c>
       <c r="D2" s="4">
-        <v>0.83972528395231905</v>
+        <v>0.900964570925326</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
       <c r="I2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H4" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
+      <c r="I7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
         <v>12</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
+      <c r="I8" t="s">
         <v>13</v>
       </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I10" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="H11" t="s">
-        <v>128</v>
-      </c>
-      <c r="I11" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0.94001318391562205</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.91293213828425102</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.96875</v>
-      </c>
-      <c r="H12" t="s">
-        <v>129</v>
-      </c>
-      <c r="I12" t="s">
-        <v>127</v>
-      </c>
-      <c r="J12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.88412017167381896</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0.91964285714285698</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.85123966942148699</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.90825688073394395</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.85344827586206895</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.97058823529411697</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.85779816513761398</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.98421052631578898</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.92941176470588205</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.86813186813186805</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>0.92532467532467499</v>
+        <v>0.929595827900912</v>
       </c>
       <c r="C18" s="4">
-        <v>0.901898734177215</v>
+        <v>0.89348370927318299</v>
       </c>
       <c r="D18" s="4">
-        <v>0.95</v>
+        <v>0.96875</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>0.90666666666666595</v>
+        <v>0.83760683760683696</v>
       </c>
       <c r="C19" s="4">
-        <v>0.87179487179487103</v>
+        <v>0.86725663716814105</v>
       </c>
       <c r="D19" s="4">
-        <v>0.94444444444444398</v>
+        <v>0.80991735537190002</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>0.98293515358361705</v>
+        <v>0.91262135922330001</v>
       </c>
       <c r="C20" s="4">
-        <v>0.97297297297297303</v>
+        <v>0.90384615384615297</v>
       </c>
       <c r="D20" s="4">
-        <v>0.99310344827586206</v>
+        <v>0.92156862745098</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>0.67128027681660896</v>
+        <v>0.93333333333333302</v>
       </c>
       <c r="C21" s="4">
-        <v>0.53005464480874298</v>
+        <v>0.87906976744186005</v>
       </c>
       <c r="D21" s="4">
-        <v>0.91509433962264097</v>
+        <v>0.99473684210526303</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4">
-        <v>0.91046658259772995</v>
+        <v>0.86338797814207602</v>
       </c>
       <c r="C22" s="4">
-        <v>0.84941176470588198</v>
+        <v>0.75961538461538403</v>
       </c>
       <c r="D22" s="4">
-        <v>0.98097826086956497</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4">
-        <v>0.92068683565004095</v>
+        <v>0.91935483870967705</v>
       </c>
       <c r="C24" s="4">
-        <v>0.88383045525902604</v>
+        <v>0.890625</v>
       </c>
       <c r="D24" s="4">
-        <v>0.96075085324232001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4">
-        <v>0.93645484949832702</v>
+        <v>0.911392405063291</v>
       </c>
       <c r="C25" s="4">
-        <v>0.93959731543624103</v>
+        <v>0.837209302325581</v>
       </c>
       <c r="D25" s="4">
-        <v>0.93333333333333302</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4">
-        <v>0.93270280101855196</v>
+        <v>0.96</v>
       </c>
       <c r="C26" s="4">
-        <v>0.88781163434902999</v>
+        <v>0.92903225806451595</v>
       </c>
       <c r="D26" s="4">
-        <v>0.98237547892720301</v>
+        <v>0.99310344827586206</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>0.86800894854586097</v>
+        <v>0.63230240549828098</v>
       </c>
       <c r="C27" s="4">
-        <v>0.85462555066079204</v>
+        <v>0.49729729729729699</v>
       </c>
       <c r="D27" s="4">
-        <v>0.88181818181818095</v>
+        <v>0.86792452830188604</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4">
-        <v>0.92356687898089096</v>
+        <v>0.84088269454123099</v>
       </c>
       <c r="C28" s="4">
-        <v>0.88957055214723901</v>
+        <v>0.73427991886409705</v>
       </c>
       <c r="D28" s="4">
-        <v>0.96026490066225101</v>
+        <v>0.98369565217391297</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4">
-        <v>0.83911671924290199</v>
+        <v>0.11764705882352899</v>
       </c>
       <c r="C29" s="4">
-        <v>0.77325581395348797</v>
+        <v>7.69230769230769E-2</v>
       </c>
       <c r="D29" s="4">
-        <v>0.917241379310344</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4">
-        <v>1</v>
+        <v>0.92976588628762502</v>
       </c>
       <c r="C30" s="4">
-        <v>1</v>
+        <v>0.91147540983606501</v>
       </c>
       <c r="D30" s="4">
-        <v>1</v>
+        <v>0.94880546075085304</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>1</v>
+        <v>0.95737704918032696</v>
       </c>
       <c r="C31" s="4">
-        <v>1</v>
+        <v>0.94193548387096704</v>
       </c>
       <c r="D31" s="4">
-        <v>1</v>
+        <v>0.97333333333333305</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4">
-        <v>0.93728222996515598</v>
+        <v>0.92700467457749003</v>
       </c>
       <c r="C32" s="4">
-        <v>0.96415770609318996</v>
+        <v>0.87330623306233002</v>
       </c>
       <c r="D32" s="4">
-        <v>0.91186440677966096</v>
+        <v>0.98773946360153198</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4">
-        <v>0.78260869565217295</v>
+        <v>0.89719626168224298</v>
       </c>
       <c r="C33" s="4">
-        <v>0.75</v>
+        <v>0.92307692307692302</v>
       </c>
       <c r="D33" s="4">
-        <v>0.81818181818181801</v>
+        <v>0.87272727272727202</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4">
-        <v>0.927152317880794</v>
+        <v>0.92499999999999905</v>
       </c>
       <c r="C34" s="4">
-        <v>0.90322580645161199</v>
+        <v>0.87573964497041401</v>
       </c>
       <c r="D34" s="4">
-        <v>0.952380952380952</v>
+        <v>0.98013245033112495</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4">
-        <v>0.59505208333333304</v>
+        <v>0.777464788732394</v>
       </c>
       <c r="C35" s="4">
-        <v>0.42590866728797699</v>
+        <v>0.65714285714285703</v>
       </c>
       <c r="D35" s="4">
-        <v>0.987041036717062</v>
+        <v>0.95172413793103405</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4">
-        <v>0.866464339908953</v>
+        <v>1</v>
       </c>
       <c r="C36" s="4">
-        <v>0.77581521739130399</v>
+        <v>1</v>
       </c>
       <c r="D36" s="4">
-        <v>0.98109965635738805</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B37" s="4">
-        <v>0</v>
+        <v>0.93333333333333302</v>
       </c>
       <c r="C37" s="4">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="D37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4">
-        <v>0.91542044618779095</v>
+        <v>0.94551845342706498</v>
       </c>
       <c r="C38" s="4">
-        <v>0.85407136322049404</v>
+        <v>0.98175182481751799</v>
       </c>
       <c r="D38" s="4">
-        <v>0.98626518753301595</v>
+        <v>0.91186440677966096</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4">
-        <v>0.94110032362459495</v>
+        <v>0.60606060606060597</v>
       </c>
       <c r="C39" s="4">
-        <v>0.93564993564993504</v>
+        <v>0.45454545454545398</v>
       </c>
       <c r="D39" s="4">
-        <v>0.94661458333333304</v>
+        <v>0.90909090909090895</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>47</v>
+      <c r="A40" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B40" s="4">
-        <v>0.99127374244266697</v>
+        <v>0.91205211726384305</v>
       </c>
       <c r="C40" s="4">
-        <v>0.99793954859734102</v>
+        <v>0.875</v>
       </c>
       <c r="D40" s="4">
-        <v>0.98469639484832505</v>
+        <v>0.952380952380952</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.61283643892339501</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.45030425963488802</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.95896328293736499</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.82446043165467597</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.70915841584158401</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.98453608247422597</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.92538783550849502</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.86669741697416902</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.99260433174854701</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0.96168582375478895</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.94360902255639101</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.98046875</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.99118608627094695</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.99857546167991895</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.98390526906783204</v>
       </c>
     </row>
   </sheetData>
@@ -2363,20 +2550,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E48E749-1D63-493F-B766-CF0D3C973D9A}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2386,13 +2576,43 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="B2" s="4">
         <v>0.87683284457477995</v>
@@ -2403,250 +2623,381 @@
       <c r="D2" s="4">
         <v>0.862863217576187</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E2" s="4">
+        <v>0.89283339969549302</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.925258855436765</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.86260367832672102</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H3" t="s">
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H4" t="s">
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
         <v>51</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
+      <c r="K7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>64</v>
+      </c>
+      <c r="K8">
         <v>8</v>
       </c>
-      <c r="I5" t="s">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
+      <c r="K9" t="s">
         <v>13</v>
       </c>
-      <c r="I8">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2662,10 +3013,14 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
@@ -2678,7 +3033,10 @@
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>0</v>
+        <v>123</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2694,67 +3052,68 @@
       <c r="D2" s="4">
         <v>0.57206200089383197</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="3"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>13</v>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I7">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
@@ -2768,7 +3127,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -2782,7 +3141,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" s="4">
         <v>0.90285714285714203</v>
@@ -2796,7 +3155,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4">
         <v>0.105263157894736</v>
@@ -2810,7 +3169,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" s="4">
         <v>0.77941176470588203</v>
@@ -2824,7 +3183,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B16" s="4">
         <v>0.868369351669941</v>
@@ -2838,7 +3197,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4">
         <v>0.77647058823529402</v>
@@ -2990,4 +3349,212 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B291F6F-B9A9-4874-ABB2-964907BBC7C5}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>